<commit_message>
removed 2D coords from 3D xlsx file
</commit_message>
<xml_diff>
--- a/mic_positions/data/3d_measured_coords.xlsx
+++ b/mic_positions/data/3d_measured_coords.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,16 +459,6 @@
           <t>Z</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>X measured</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Y measured</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -493,12 +483,6 @@
       <c r="F2" t="n">
         <v>0.02</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.649</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.02</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -523,12 +507,6 @@
       <c r="F3" t="n">
         <v>0.266</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.902</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.266</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -553,12 +531,6 @@
       <c r="F4" t="n">
         <v>0.287</v>
       </c>
-      <c r="G4" t="n">
-        <v>0.251</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.287</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -583,12 +555,6 @@
       <c r="F5" t="n">
         <v>0.38</v>
       </c>
-      <c r="G5" t="n">
-        <v>1.313</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.38</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -613,12 +579,6 @@
       <c r="F6" t="n">
         <v>0.425</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.5620000000000001</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.425</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -643,12 +603,6 @@
       <c r="F7" t="n">
         <v>0.629</v>
       </c>
-      <c r="G7" t="n">
-        <v>0.904</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.629</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -673,12 +627,6 @@
       <c r="F8" t="n">
         <v>0.672</v>
       </c>
-      <c r="G8" t="n">
-        <v>0.137</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.672</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -703,12 +651,6 @@
       <c r="F9" t="n">
         <v>0.718</v>
       </c>
-      <c r="G9" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.718</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -733,12 +675,6 @@
       <c r="F10" t="n">
         <v>0.774</v>
       </c>
-      <c r="G10" t="n">
-        <v>0.542</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.774</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -763,12 +699,6 @@
       <c r="F11" t="n">
         <v>0.989</v>
       </c>
-      <c r="G11" t="n">
-        <v>0.289</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.989</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -793,12 +723,6 @@
       <c r="F12" t="n">
         <v>1.148</v>
       </c>
-      <c r="G12" t="n">
-        <v>1.085</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1.148</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -823,12 +747,6 @@
       <c r="F13" t="n">
         <v>1.194</v>
       </c>
-      <c r="G13" t="n">
-        <v>0.724</v>
-      </c>
-      <c r="H13" t="n">
-        <v>1.194</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -853,12 +771,6 @@
       <c r="F14" t="n">
         <v>1.257</v>
       </c>
-      <c r="G14" t="n">
-        <v>0.07199999999999999</v>
-      </c>
-      <c r="H14" t="n">
-        <v>1.257</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -883,12 +795,6 @@
       <c r="F15" t="n">
         <v>1.372</v>
       </c>
-      <c r="G15" t="n">
-        <v>0.451</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1.372</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -913,12 +819,6 @@
       <c r="F16" t="n">
         <v>1.485</v>
       </c>
-      <c r="G16" t="n">
-        <v>0.959</v>
-      </c>
-      <c r="H16" t="n">
-        <v>1.485</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -943,12 +843,6 @@
       <c r="F17" t="n">
         <v>1.51</v>
       </c>
-      <c r="G17" t="n">
-        <v>1.307</v>
-      </c>
-      <c r="H17" t="n">
-        <v>1.51</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -973,12 +867,6 @@
       <c r="F18" t="n">
         <v>1.689</v>
       </c>
-      <c r="G18" t="n">
-        <v>0.589</v>
-      </c>
-      <c r="H18" t="n">
-        <v>1.689</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1003,12 +891,6 @@
       <c r="F19" t="n">
         <v>0.023</v>
       </c>
-      <c r="G19" t="n">
-        <v>0.649</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.023</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1033,12 +915,6 @@
       <c r="F20" t="n">
         <v>0.267</v>
       </c>
-      <c r="G20" t="n">
-        <v>0.903</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.267</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1063,12 +939,6 @@
       <c r="F21" t="n">
         <v>0.287</v>
       </c>
-      <c r="G21" t="n">
-        <v>0.251</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.287</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1093,12 +963,6 @@
       <c r="F22" t="n">
         <v>0.38</v>
       </c>
-      <c r="G22" t="n">
-        <v>1.312</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.38</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1123,12 +987,6 @@
       <c r="F23" t="n">
         <v>0.425</v>
       </c>
-      <c r="G23" t="n">
-        <v>0.5610000000000001</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.425</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1153,12 +1011,6 @@
       <c r="F24" t="n">
         <v>0.63</v>
       </c>
-      <c r="G24" t="n">
-        <v>0.904</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.63</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1183,12 +1035,6 @@
       <c r="F25" t="n">
         <v>0.675</v>
       </c>
-      <c r="G25" t="n">
-        <v>0.136</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.675</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1213,12 +1059,6 @@
       <c r="F26" t="n">
         <v>0.717</v>
       </c>
-      <c r="G26" t="n">
-        <v>1.231</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.717</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1243,12 +1083,6 @@
       <c r="F27" t="n">
         <v>0.773</v>
       </c>
-      <c r="G27" t="n">
-        <v>0.542</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0.773</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1273,12 +1107,6 @@
       <c r="F28" t="n">
         <v>0.99</v>
       </c>
-      <c r="G28" t="n">
-        <v>0.289</v>
-      </c>
-      <c r="H28" t="n">
-        <v>0.99</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1303,12 +1131,6 @@
       <c r="F29" t="n">
         <v>1.15</v>
       </c>
-      <c r="G29" t="n">
-        <v>1.084</v>
-      </c>
-      <c r="H29" t="n">
-        <v>1.15</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1333,12 +1155,6 @@
       <c r="F30" t="n">
         <v>1.194</v>
       </c>
-      <c r="G30" t="n">
-        <v>0.721</v>
-      </c>
-      <c r="H30" t="n">
-        <v>1.194</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1363,12 +1179,6 @@
       <c r="F31" t="n">
         <v>1.261</v>
       </c>
-      <c r="G31" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="H31" t="n">
-        <v>1.261</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1393,12 +1203,6 @@
       <c r="F32" t="n">
         <v>1.375</v>
       </c>
-      <c r="G32" t="n">
-        <v>0.451</v>
-      </c>
-      <c r="H32" t="n">
-        <v>1.375</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1423,12 +1227,6 @@
       <c r="F33" t="n">
         <v>1.485</v>
       </c>
-      <c r="G33" t="n">
-        <v>0.969</v>
-      </c>
-      <c r="H33" t="n">
-        <v>1.485</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1453,12 +1251,6 @@
       <c r="F34" t="n">
         <v>1.508</v>
       </c>
-      <c r="G34" t="n">
-        <v>1.303</v>
-      </c>
-      <c r="H34" t="n">
-        <v>1.508</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1483,12 +1275,6 @@
       <c r="F35" t="n">
         <v>1.691</v>
       </c>
-      <c r="G35" t="n">
-        <v>0.589</v>
-      </c>
-      <c r="H35" t="n">
-        <v>1.691</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1513,12 +1299,6 @@
       <c r="F36" t="n">
         <v>0.023</v>
       </c>
-      <c r="G36" t="n">
-        <v>0.649</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0.023</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1543,12 +1323,6 @@
       <c r="F37" t="n">
         <v>0.27</v>
       </c>
-      <c r="G37" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0.27</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1573,12 +1347,6 @@
       <c r="F38" t="n">
         <v>0.289</v>
       </c>
-      <c r="G38" t="n">
-        <v>0.251</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.289</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1603,12 +1371,6 @@
       <c r="F39" t="n">
         <v>0.385</v>
       </c>
-      <c r="G39" t="n">
-        <v>1.312</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0.385</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1633,12 +1395,6 @@
       <c r="F40" t="n">
         <v>0.427</v>
       </c>
-      <c r="G40" t="n">
-        <v>0.5610000000000001</v>
-      </c>
-      <c r="H40" t="n">
-        <v>0.427</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1663,12 +1419,6 @@
       <c r="F41" t="n">
         <v>0.63</v>
       </c>
-      <c r="G41" t="n">
-        <v>0.904</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0.63</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1693,12 +1443,6 @@
       <c r="F42" t="n">
         <v>0.677</v>
       </c>
-      <c r="G42" t="n">
-        <v>0.135</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0.677</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1723,12 +1467,6 @@
       <c r="F43" t="n">
         <v>0.72</v>
       </c>
-      <c r="G43" t="n">
-        <v>1.229</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0.72</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1753,12 +1491,6 @@
       <c r="F44" t="n">
         <v>0.773</v>
       </c>
-      <c r="G44" t="n">
-        <v>0.541</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0.773</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1783,12 +1515,6 @@
       <c r="F45" t="n">
         <v>0.99</v>
       </c>
-      <c r="G45" t="n">
-        <v>0.289</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0.99</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1813,12 +1539,6 @@
       <c r="F46" t="n">
         <v>1.149</v>
       </c>
-      <c r="G46" t="n">
-        <v>1.082</v>
-      </c>
-      <c r="H46" t="n">
-        <v>1.149</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1843,12 +1563,6 @@
       <c r="F47" t="n">
         <v>1.195</v>
       </c>
-      <c r="G47" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="H47" t="n">
-        <v>1.195</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1873,12 +1587,6 @@
       <c r="F48" t="n">
         <v>1.26</v>
       </c>
-      <c r="G48" t="n">
-        <v>0.074</v>
-      </c>
-      <c r="H48" t="n">
-        <v>1.26</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1903,12 +1611,6 @@
       <c r="F49" t="n">
         <v>1.375</v>
       </c>
-      <c r="G49" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="H49" t="n">
-        <v>1.375</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1933,12 +1635,6 @@
       <c r="F50" t="n">
         <v>1.485</v>
       </c>
-      <c r="G50" t="n">
-        <v>0.963</v>
-      </c>
-      <c r="H50" t="n">
-        <v>1.485</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1963,12 +1659,6 @@
       <c r="F51" t="n">
         <v>1.511</v>
       </c>
-      <c r="G51" t="n">
-        <v>1.305</v>
-      </c>
-      <c r="H51" t="n">
-        <v>1.511</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1993,12 +1683,6 @@
       <c r="F52" t="n">
         <v>1.69</v>
       </c>
-      <c r="G52" t="n">
-        <v>0.589</v>
-      </c>
-      <c r="H52" t="n">
-        <v>1.69</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2023,12 +1707,6 @@
       <c r="F53" t="n">
         <v>1.871</v>
       </c>
-      <c r="G53" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="H53" t="n">
-        <v>0.05299999999999994</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2053,12 +1731,6 @@
       <c r="F54" t="n">
         <v>1.871</v>
       </c>
-      <c r="G54" t="n">
-        <v>0.3109999999999999</v>
-      </c>
-      <c r="H54" t="n">
-        <v>0.152</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2083,12 +1755,6 @@
       <c r="F55" t="n">
         <v>1.871</v>
       </c>
-      <c r="G55" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H55" t="n">
-        <v>0.172</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2113,12 +1779,6 @@
       <c r="F56" t="n">
         <v>1.871</v>
       </c>
-      <c r="G56" t="n">
-        <v>0.09399999999999997</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0.4349999999999999</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2143,12 +1803,6 @@
       <c r="F57" t="n">
         <v>1.871</v>
       </c>
-      <c r="G57" t="n">
-        <v>0.4419999999999999</v>
-      </c>
-      <c r="H57" t="n">
-        <v>0.4419999999999999</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2173,12 +1827,6 @@
       <c r="F58" t="n">
         <v>1.871</v>
       </c>
-      <c r="G58" t="n">
-        <v>1.059</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0.4429999999999999</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2203,12 +1851,6 @@
       <c r="F59" t="n">
         <v>1.871</v>
       </c>
-      <c r="G59" t="n">
-        <v>0.715</v>
-      </c>
-      <c r="H59" t="n">
-        <v>0.489</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2233,12 +1875,6 @@
       <c r="F60" t="n">
         <v>1.871</v>
       </c>
-      <c r="G60" t="n">
-        <v>0.496</v>
-      </c>
-      <c r="H60" t="n">
-        <v>0.751</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2263,12 +1899,6 @@
       <c r="F61" t="n">
         <v>1.871</v>
       </c>
-      <c r="G61" t="n">
-        <v>0.06499999999999995</v>
-      </c>
-      <c r="H61" t="n">
-        <v>0.778</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2293,12 +1923,6 @@
       <c r="F62" t="n">
         <v>1.871</v>
       </c>
-      <c r="G62" t="n">
-        <v>0.7899999999999999</v>
-      </c>
-      <c r="H62" t="n">
-        <v>0.9059999999999999</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2323,12 +1947,6 @@
       <c r="F63" t="n">
         <v>1.871</v>
       </c>
-      <c r="G63" t="n">
-        <v>0.485</v>
-      </c>
-      <c r="H63" t="n">
-        <v>1.144</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2353,12 +1971,6 @@
       <c r="F64" t="n">
         <v>1.871</v>
       </c>
-      <c r="G64" t="n">
-        <v>1.138</v>
-      </c>
-      <c r="H64" t="n">
-        <v>1.17</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2382,12 +1994,6 @@
       </c>
       <c r="F65" t="n">
         <v>1.871</v>
-      </c>
-      <c r="G65" t="n">
-        <v>0.198</v>
-      </c>
-      <c r="H65" t="n">
-        <v>1.182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switched left & right again
</commit_message>
<xml_diff>
--- a/mic_positions/data/3d_measured_coords.xlsx
+++ b/mic_positions/data/3d_measured_coords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fulbr\OneDrive\Documents\01 Uni OneDrive\13 WiSe 2425\02 MAP Microphone Array Project\Bassoon Project\02 Code\Bassoon2425\mic_positions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A8B68F-E059-417B-B6AC-1562CFACE385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D748F8-4609-41A0-92BF-2A5AB232419D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="12390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -603,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -634,7 +634,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>1.37</v>
@@ -654,7 +654,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>1.37</v>
@@ -674,7 +674,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>1.37</v>
@@ -694,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>1.37</v>
@@ -714,7 +714,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>1.37</v>
@@ -734,7 +734,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>1.37</v>
@@ -754,7 +754,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>1.37</v>
@@ -774,7 +774,7 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>1.37</v>
@@ -794,7 +794,7 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>1.37</v>
@@ -814,7 +814,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D11">
         <v>1.37</v>
@@ -834,7 +834,7 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>1.37</v>
@@ -854,7 +854,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>1.37</v>
@@ -874,7 +874,7 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D14">
         <v>1.37</v>
@@ -894,7 +894,7 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D15">
         <v>1.37</v>
@@ -914,7 +914,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D16">
         <v>1.37</v>
@@ -934,7 +934,7 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1.37</v>
@@ -954,7 +954,7 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>1.37</v>
@@ -1314,7 +1314,7 @@
         <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D36">
         <v>2.8000000000000001E-2</v>
@@ -1334,7 +1334,7 @@
         <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D37">
         <v>2.8000000000000001E-2</v>
@@ -1354,7 +1354,7 @@
         <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D38">
         <v>2.8000000000000001E-2</v>
@@ -1374,7 +1374,7 @@
         <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D39">
         <v>2.8000000000000001E-2</v>
@@ -1394,7 +1394,7 @@
         <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D40">
         <v>2.8000000000000001E-2</v>
@@ -1414,7 +1414,7 @@
         <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D41">
         <v>2.8000000000000001E-2</v>
@@ -1434,7 +1434,7 @@
         <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D42">
         <v>2.8000000000000001E-2</v>
@@ -1454,7 +1454,7 @@
         <v>49</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D43">
         <v>2.8000000000000001E-2</v>
@@ -1474,7 +1474,7 @@
         <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D44">
         <v>2.8000000000000001E-2</v>
@@ -1494,7 +1494,7 @@
         <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D45">
         <v>2.8000000000000001E-2</v>
@@ -1514,7 +1514,7 @@
         <v>52</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D46">
         <v>2.8000000000000001E-2</v>
@@ -1534,7 +1534,7 @@
         <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D47">
         <v>2.8000000000000001E-2</v>
@@ -1554,7 +1554,7 @@
         <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D48">
         <v>2.8000000000000001E-2</v>
@@ -1574,7 +1574,7 @@
         <v>55</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D49">
         <v>2.8000000000000001E-2</v>
@@ -1594,7 +1594,7 @@
         <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D50">
         <v>2.8000000000000001E-2</v>
@@ -1614,7 +1614,7 @@
         <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D51">
         <v>2.8000000000000001E-2</v>
@@ -1634,7 +1634,7 @@
         <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D52">
         <v>2.8000000000000001E-2</v>

</xml_diff>